<commit_message>
update prepayment functions, install Rotativa
</commit_message>
<xml_diff>
--- a/Trojantrading/wwwroot/ImportUsers.xlsx
+++ b/Trojantrading/wwwroot/ImportUsers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William.Deng\Desktop\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B8054B1-F05D-489C-9B8F-EC8D1ED2AE7C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4A61E74-092E-44CC-887F-7B1D49588B66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>

</xml_diff>